<commit_message>
thickened USB sig traces, centered footprints, and other small changes
</commit_message>
<xml_diff>
--- a/bom/DFTBoardBOM.xlsx
+++ b/bom/DFTBoardBOM.xlsx
@@ -259,7 +259,7 @@
     <t xml:space="preserve">http://www.digikey.com/product-detail/en/kemet/C0402C150J4GACTU/399-8947-1-ND/3522464</t>
   </si>
   <si>
-    <t xml:space="preserve">C53 C87 </t>
+    <t xml:space="preserve">C53 C87 C152</t>
   </si>
   <si>
     <t xml:space="preserve">2.2uF</t>
@@ -1149,21 +1149,21 @@
   </sheetPr>
   <dimension ref="A1:M78"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I25" activeCellId="0" sqref="I25"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="31.8571428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="8.63775510204082"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="31.8571428571429"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="8.63775510204082"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="23.7602040816327"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="1" width="31.8571428571429"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="31.4540816326531"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="31.4540816326531"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="23.3520408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="1" width="31.4540816326531"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1675,12 +1675,12 @@
       <c r="L17" s="0"/>
       <c r="M17" s="0"/>
     </row>
-    <row r="18" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
         <v>79</v>
       </c>
       <c r="B18" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>80</v>
@@ -1696,7 +1696,7 @@
       </c>
       <c r="G18" s="1" t="n">
         <f aca="false">F18*B18</f>
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>82</v>
@@ -3436,7 +3436,7 @@
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G78" s="1" t="n">
         <f aca="false">SUM(G2:G77)</f>
-        <v>215.2</v>
+        <v>215.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>